<commit_message>
add new data sheet to excel for testing
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/HrmTestData.xlsx
+++ b/src/test/resources/testdata/HrmTestData.xlsx
@@ -3,17 +3,18 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Employee" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="NegativeLogins" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Firstname</t>
   </si>
@@ -55,6 +56,42 @@
   </si>
   <si>
     <t>muhammadali</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>errorMessage</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>admin12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid credentials</t>
+  </si>
+  <si>
+    <t>Admi</t>
+  </si>
+  <si>
+    <t>admin123</t>
+  </si>
+  <si>
+    <t>admin14</t>
+  </si>
+  <si>
+    <t>admin15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Username cannot be empty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Password cannot be empty</t>
   </si>
 </sst>
 </file>
@@ -127,7 +164,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -138,6 +175,7 @@
     <xf fontId="2" fillId="2" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -719,4 +757,100 @@
   <pageSetup paperSize="9" scale="100" firstPageNumber="2147483647" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col bestFit="1" min="2" max="2" width="8.86328125"/>
+    <col bestFit="1" min="3" max="3" width="24.34375"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="4"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="4"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="4"/>
+    </row>
+  </sheetData>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="4294967295" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
some web elements were changed, causing tests to fail, fixed them
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/HrmTestData.xlsx
+++ b/src/test/resources/testdata/HrmTestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shahnoza/IdeaProjects/HRMFramework/src/test/resources/testdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IntelliJ_IDEA_Projects\TestNGFramework\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A83B02D5-EFDC-B34A-A7BF-A8BBA2FC027C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2373A26F-ED39-4A91-86E3-C661A9E500D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="620" yWindow="3520" windowWidth="27200" windowHeight="14380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21920" yWindow="-21710" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Employee" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
     <t>Firstname</t>
   </si>
@@ -86,12 +86,6 @@
     <t>admin15</t>
   </si>
   <si>
-    <t>Username cannot be empty</t>
-  </si>
-  <si>
-    <t>Password cannot be empty</t>
-  </si>
-  <si>
     <t>Luke</t>
   </si>
   <si>
@@ -99,13 +93,16 @@
   </si>
   <si>
     <t>lukesky</t>
+  </si>
+  <si>
+    <t>Required</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -417,19 +414,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.8203125" defaultRowHeight="14.35"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.8203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.64453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -443,7 +440,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -457,7 +454,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -471,15 +468,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>7</v>
@@ -495,16 +492,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.8203125" defaultRowHeight="14.35"/>
   <cols>
-    <col min="3" max="3" width="24.33203125" bestFit="1"/>
+    <col min="3" max="3" width="24.3515625" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -515,7 +512,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" s="4" t="s">
         <v>14</v>
       </c>
@@ -527,7 +524,7 @@
       </c>
       <c r="D2" s="4"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" s="4" t="s">
         <v>17</v>
       </c>
@@ -539,7 +536,7 @@
       </c>
       <c r="D3" s="4"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" s="4" t="s">
         <v>17</v>
       </c>
@@ -551,31 +548,31 @@
       </c>
       <c r="D4" s="4"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" s="4"/>
       <c r="B5" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D6" s="4"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D7" s="4"/>
     </row>

</xml_diff>